<commit_message>
mapping in snapgene is ok
</commit_message>
<xml_diff>
--- a/tests/T2/T2_out/eblocks-plate-upload-template-96-filled.xlsx
+++ b/tests/T2/T2_out/eblocks-plate-upload-template-96-filled.xlsx
@@ -458,12 +458,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Y77S_Block-0</t>
+          <t>P80-S106_Block-0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ggagatgcctgccatcggcatgaccgaccacgggaacatgttcggcgccagcgagttctacaactcggcgaccaaggccggcatcaaacccatcatcgggatcgaggcctcgatcgcgcccggttcccggttcgacaccaagcgcgtcacatggggcgacccgggccagaagggcgacgacgtctccggcagcggtgcgtacacgcacatgacgatggtcgccgagaacgcgacgggcctgcgcaacctgttcaagctgtcctcgctggcgtcgttcgaggggcagctgggcaagtggtcgcgtatggacgccgagatcatcgccgagcacgccgagggcatcatcgccaccaccggctgcccgtcgggcgaggtccagacccgcctgcgcctcggccacgagcgcgaggcgctcgaagccgcggcgaagtggcgcgagatcttcggcccggagaacttcttcctcgaactgatggaccacggtctcgacatcgagcgccgggtccgcgagggcctgctggagatcggccgcaagctcggcatcccgccgctggccaccaacgactgtcactacgtcacgcgtgaggccgcacgcaaccacgaggcgctgctgtgtgtgcagacgggcaagaccctctcggatcccacgcggttcaagttcgacggtgacggctacttcctcaagt</t>
+          <t>acccatcatcgggatcgaggcctacatcgcggcgtacacgcacatgacgatggtcgccgagaacgcgacgggcctgcgcaacctgttcaagctgtcctcgctggcgtcgttcgaggggcagctgggcaagtggtcgcgtatggacgccgagatcatcgccgagcacgccgagggcatcatcgccaccaccggctgcccgtcgggcgaggtccagacccgcctgcgcctcggccacgagcgcgaggcgctcgaagccgcggcgaagtggcgcgagatcttcggcccggagaacttcttcctcgaactgatggaccacggtctcgacatcgagcgccgggtccgcgagggcctgctggagatcggccgcaagctcggcatcccgccgctggccaccaacgactgtcactacgtcacgcgtgaggccgcacgcaaccacgaggcgctgctgtgtgtgcagacgggcaagaccctctcggatcccacgcggttcaagttcgacggtgacggctacttcctcaagt</t>
         </is>
       </c>
     </row>
@@ -475,12 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Y107G_Block-0</t>
+          <t>Y77S_Block-0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ggagatgcctgccatcggcatgaccgaccacgggaacatgttcggcgccagcgagttctacaactcggcgaccaaggccggcatcaaacccatcatcgggatcgaggcctacatcgcgcccggttcccggttcgacaccaagcgcgtcacatggggcgacccgggccagaagggcgacgacgtctccggcagcggtgcgggcacgcacatgacgatggtcgccgagaacgcgacgggcctgcgcaacctgttcaagctgtcctcgctggcgtcgttcgaggggcagctgggcaagtggtcgcgtatggacgccgagatcatcgccgagcacgccgagggcatcatcgccaccaccggctgcccgtcgggcgaggtccagacccgcctgcgcctcggccacgagcgcgaggcgctcgaagccgcggcgaagtggcgcgagatcttcggcccggagaacttcttcctcgaactgatggaccacggtctcgacatcgagcgccgggtccgcgagggcctgctggagatcggccgcaagctcggcatcccgccgctggccaccaacgactgtcactacgtcacgcgtgaggccgcacgcaaccacgaggcgctgctgtgtgtgcagacgggcaagaccctctcggatcccacgcggttcaagttcgacggtgacggctacttcctcaagt</t>
+          <t>acccatcatcgggatcgaggcctcgatcgcgcccggttcccggttcgacaccaagcgcgtcacatggggcgacccgggccagaagggcgacgacgtctccggcagcggtgcgtacacgcacatgacgatggtcgccgagaacgcgacgggcctgcgcaacctgttcaagctgtcctcgctggcgtcgttcgaggggcagctgggcaagtggtcgcgtatggacgccgagatcatcgccgagcacgccgagggcatcatcgccaccaccggctgcccgtcgggcgaggtccagacccgcctgcgcctcggccacgagcgcgaggcgctcgaagccgcggcgaagtggcgcgagatcttcggcccggagaacttcttcctcgaactgatggaccacggtctcgacatcgagcgccgggtccgcgagggcctgctggagatcggccgcaagctcggcatcccgccgctggccaccaacgactgtcactacgtcacgcgtgaggccgcacgcaaccacgaggcgctgctgtgtgtgcagacgggcaagaccctctcggatcccacgcggttcaagttcgacggtgacggctacttcctcaagt</t>
         </is>
       </c>
     </row>
@@ -492,12 +492,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>W139F_Block-0</t>
+          <t>Y107G_Block-0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ggagatgcctgccatcggcatgaccgaccacgggaacatgttcggcgccagcgagttctacaactcggcgaccaaggccggcatcaaacccatcatcgggatcgaggcctacatcgcgcccggttcccggttcgacaccaagcgcgtcacatggggcgacccgggccagaagggcgacgacgtctccggcagcggtgcgtacacgcacatgacgatggtcgccgagaacgcgacgggcctgcgcaacctgttcaagctgtcctcgctggcgtcgttcgaggggcagctgggcaagttctcgcgtatggacgccgagatcatcgccgagcacgccgagggcatcatcgccaccaccggctgcccgtcgggcgaggtccagacccgcctgcgcctcggccacgagcgcgaggcgctcgaagccgcggcgaagtggcgcgagatcttcggcccggagaacttcttcctcgaactgatggaccacggtctcgacatcgagcgccgggtccgcgagggcctgctggagatcggccgcaagctcggcatcccgccgctggccaccaacgactgtcactacgtcacgcgtgaggccgcacgcaaccacgaggcgctgctgtgtgtgcagacgggcaagaccctctcggatcccacgcggttcaagttcgacggtgacggctacttcctcaagt</t>
+          <t>acccatcatcgggatcgaggcctacatcgcgcccggttcccggttcgacaccaagcgcgtcacatggggcgacccgggccagaagggcgacgacgtctccggcagcggtgcgggcacgcacatgacgatggtcgccgagaacgcgacgggcctgcgcaacctgttcaagctgtcctcgctggcgtcgttcgaggggcagctgggcaagtggtcgcgtatggacgccgagatcatcgccgagcacgccgagggcatcatcgccaccaccggctgcccgtcgggcgaggtccagacccgcctgcgcctcggccacgagcgcgaggcgctcgaagccgcggcgaagtggcgcgagatcttcggcccggagaacttcttcctcgaactgatggaccacggtctcgacatcgagcgccgggtccgcgagggcctgctggagatcggccgcaagctcggcatcccgccgctggccaccaacgactgtcactacgtcacgcgtgaggccgcacgcaaccacgaggcgctgctgtgtgtgcagacgggcaagaccctctcggatcccacgcggttcaagttcgacggtgacggctacttcctcaagt</t>
         </is>
       </c>
     </row>
@@ -509,12 +509,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>D228G_Block-0</t>
+          <t>W139F_Block-0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ggagatgcctgccatcggcatgaccgaccacgggaacatgttcggcgccagcgagttctacaactcggcgaccaaggccggcatcaaacccatcatcgggatcgaggcctacatcgcgcccggttcccggttcgacaccaagcgcgtcacatggggcgacccgggccagaagggcgacgacgtctccggcagcggtgcgtacacgcacatgacgatggtcgccgagaacgcgacgggcctgcgcaacctgttcaagctgtcctcgctggcgtcgttcgaggggcagctgggcaagtggtcgcgtatggacgccgagatcatcgccgagcacgccgagggcatcatcgccaccaccggctgcccgtcgggcgaggtccagacccgcctgcgcctcggccacgagcgcgaggcgctcgaagccgcggcgaagtggcgcgagatcttcggcccggagaacttcttcctcgaactgatggaccacggtctcgacatcgagcgccgggtccgcgagggcctgctggagatcggccgcaagctcggcatcccgccgctggccaccaacggctgtcactacgtcacgcgtgaggccgcacgcaaccacgaggcgctgctgtgtgtgcagacgggcaagaccctctcggatcccacgcggttcaagttcgacggtgacggctacttcctcaagt</t>
+          <t>acccatcatcgggatcgaggcctacatcgcgcccggttcccggttcgacaccaagcgcgtcacatggggcgacccgggccagaagggcgacgacgtctccggcagcggtgcgtacacgcacatgacgatggtcgccgagaacgcgacgggcctgcgcaacctgttcaagctgtcctcgctggcgtcgttcgaggggcagctgggcaagttctcgcgtatggacgccgagatcatcgccgagcacgccgagggcatcatcgccaccaccggctgcccgtcgggcgaggtccagacccgcctgcgcctcggccacgagcgcgaggcgctcgaagccgcggcgaagtggcgcgagatcttcggcccggagaacttcttcctcgaactgatggaccacggtctcgacatcgagcgccgggtccgcgagggcctgctggagatcggccgcaagctcggcatcccgccgctggccaccaacgactgtcactacgtcacgcgtgaggccgcacgcaaccacgaggcgctgctgtgtgtgcagacgggcaagaccctctcggatcccacgcggttcaagttcgacggtgacggctacttcctcaagt</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>F260A_Block-0</t>
+          <t>D228G_Block-0</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ggagatgcctgccatcggcatgaccgaccacgggaacatgttcggcgccagcgagttctacaactcggcgaccaaggccggcatcaaacccatcatcgggatcgaggcctacatcgcgcccggttcccggttcgacaccaagcgcgtcacatggggcgacccgggccagaagggcgacgacgtctccggcagcggtgcgtacacgcacatgacgatggtcgccgagaacgcgacgggcctgcgcaacctgttcaagctgtcctcgctggcgtcgttcgaggggcagctgggcaagtggtcgcgtatggacgccgagatcatcgccgagcacgccgagggcatcatcgccaccaccggctgcccgtcgggcgaggtccagacccgcctgcgcctcggccacgagcgcgaggcgctcgaagccgcggcgaagtggcgcgagatcttcggcccggagaacttcttcctcgaactgatggaccacggtctcgacatcgagcgccgggtccgcgagggcctgctggagatcggccgcaagctcggcatcccgccgctggccaccaacgactgtcactacgtcacgcgtgaggccgcacgcaaccacgaggcgctgctgtgtgtgcagacgggcaagaccctctcggatcccacgcggttcaaggccgacggtgacggctacttcctcaagt</t>
+          <t>acccatcatcgggatcgaggcctacatcgcgcccggttcccggttcgacaccaagcgcgtcacatggggcgacccgggccagaagggcgacgacgtctccggcagcggtgcgtacacgcacatgacgatggtcgccgagaacgcgacgggcctgcgcaacctgttcaagctgtcctcgctggcgtcgttcgaggggcagctgggcaagtggtcgcgtatggacgccgagatcatcgccgagcacgccgagggcatcatcgccaccaccggctgcccgtcgggcgaggtccagacccgcctgcgcctcggccacgagcgcgaggcgctcgaagccgcggcgaagtggcgcgagatcttcggcccggagaacttcttcctcgaactgatggaccacggtctcgacatcgagcgccgggtccgcgagggcctgctggagatcggccgcaagctcggcatcccgccgctggccaccaacggctgtcactacgtcacgcgtgaggccgcacgcaaccacgaggcgctgctgtgtgtgcagacgggcaagaccctctcggatcccacgcggttcaagttcgacggtgacggctacttcctcaagt</t>
         </is>
       </c>
     </row>
@@ -543,12 +543,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>I599A-I600L_Block-2</t>
+          <t>F260A_Block-0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>caacccggagcgtccgtccgcgcccgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacggccctgggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
+          <t>acccatcatcgggatcgaggcctacatcgcgcccggttcccggttcgacaccaagcgcgtcacatggggcgacccgggccagaagggcgacgacgtctccggcagcggtgcgtacacgcacatgacgatggtcgccgagaacgcgacgggcctgcgcaacctgttcaagctgtcctcgctggcgtcgttcgaggggcagctgggcaagtggtcgcgtatggacgccgagatcatcgccgagcacgccgagggcatcatcgccaccaccggctgcccgtcgggcgaggtccagacccgcctgcgcctcggccacgagcgcgaggcgctcgaagccgcggcgaagtggcgcgagatcttcggcccggagaacttcttcctcgaactgatggaccacggtctcgacatcgagcgccgggtccgcgagggcctgctggagatcggccgcaagctcggcatcccgccgctggccaccaacgactgtcactacgtcacgcgtgaggccgcacgcaaccacgaggcgctgctgtgtgtgcagacgggcaagaccctctcggatcccacgcggttcaaggccgacggtgacggctacttcctcaagt</t>
         </is>
       </c>
     </row>
@@ -560,12 +560,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>M813C_Block-4</t>
+          <t>I599A-I600L_Block-2</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ggccaactatccggccgagtactgcgcaggcctgctcacctcggtcggtgacgacaaggacaaggccgcggtctacctggcggactgccggcgcctgggcatcacggtgctgccgccggacgtcaacgagtcggagcacaacttcgcctcggtcggcgacgacatccgattcggcctcggcgccatccgcaacgtcggcgccaacgtcgtctcgtcactgatcaagacccgcaccgagaagggcaagttcaccgacttctcggactacctcaacaagatcgacatcacggcctgcaacaagaaggtcaccgaatcgctgatcaaggcgggcgctttcgattcgttggggcatccgcgcaagggcctgttcctggtgcacaccgacgccgtcgactcggtgctgggtaccaagaaggccgaggcgatggggcagttcgacctgttcgggggcggcgagg</t>
+          <t>cgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacggccctgggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
         </is>
       </c>
     </row>
@@ -577,12 +577,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>H851A_Block-4</t>
+          <t>M813C_Block-4</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ggccaactatccggccgagtacatggcaggcctgctcacctcggtcggtgacgacaaggacaaggccgcggtctacctggcggactgccggcgcctgggcatcacggtgctgccgccggacgtcaacgagtcggaggccaacttcgcctcggtcggcgacgacatccgattcggcctcggcgccatccgcaacgtcggcgccaacgtcgtctcgtcactgatcaagacccgcaccgagaagggcaagttcaccgacttctcggactacctcaacaagatcgacatcacggcctgcaacaagaaggtcaccgaatcgctgatcaaggcgggcgctttcgattcgttggggcatccgcgcaagggcctgttcctggtgcacaccgacgccgtcgactcggtgctgggtaccaagaaggccgaggcgatggggcagttcgacctgttcgggggcggcgagg</t>
+          <t>ggccaactatccggccgagtactgcgcaggcctgctcacctcggtcggtgacgacaaggacaaggccgcggtctacctggcggactgccggcgcctgggcatcacggtgctgccgccggacgtcaacgagtcggagcacaacttcgcctcggtcggcgacgacatccgattcggcctcggcgccatccgcaacgtcggcgccaacgtcgtctcgtcactgatcaagacccgcaccgagaagggcaagttcaccgacttctcggactacctcaacaagatcgacatcacggcctgcaacaagaaggtcaccgaatcgctgatcaaggcgggcgctttcgattcgttggggcatccgcgcaagggcctgttcctggtgcacaccgacgccgtcgactcggtgctgggtaccaagaaggccgaggcgatggggcagttcgacctgttcgggggcggcgagg</t>
         </is>
       </c>
     </row>
@@ -594,12 +594,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Q949A_Block-4</t>
+          <t>H851A_Block-4</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ggccaactatccggccgagtacatggcaggcctgctcacctcggtcggtgacgacaaggacaaggccgcggtctacctggcggactgccggcgcctgggcatcacggtgctgccgccggacgtcaacgagtcggagcacaacttcgcctcggtcggcgacgacatccgattcggcctcggcgccatccgcaacgtcggcgccaacgtcgtctcgtcactgatcaagacccgcaccgagaagggcaagttcaccgacttctcggactacctcaacaagatcgacatcacggcctgcaacaagaaggtcaccgaatcgctgatcaaggcgggcgctttcgattcgttggggcatccgcgcaagggcctgttcctggtgcacaccgacgccgtcgactcggtgctgggtaccaagaaggccgaggcgatgggggccttcgacctgttcgggggcggcgagg</t>
+          <t>ggccaactatccggccgagtacatggcaggcctgctcacctcggtcggtgacgacaaggacaaggccgcggtctacctggcggactgccggcgcctgggcatcacggtgctgccgccggacgtcaacgagtcggaggccaacttcgcctcggtcggcgacgacatccgattcggcctcggcgccatccgcaacgtcggcgccaacgtcgtctcgtcactgatcaagacccgcaccgagaagggcaagttcaccgacttctcggactacctcaacaagatcgacatcacggcctgcaacaagaaggtcaccgaatcgctgatcaaggcgggcgctttcgattcgttggggcatccgcgcaagggcctgttcctggtgcacaccgacgccgtcgactcggtgctgggtaccaagaaggccgaggcgatggggcagttcgacctgttcgggggcggcgagg</t>
         </is>
       </c>
     </row>
@@ -611,12 +611,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>F473G_Block-2</t>
+          <t>Q949A_Block-4</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>caacccggagcgtccgtccgcgcccgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacggcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
+          <t>ggccaactatccggccgagtacatggcaggcctgctcacctcggtcggtgacgacaaggacaaggccgcggtctacctggcggactgccggcgcctgggcatcacggtgctgccgccggacgtcaacgagtcggagcacaacttcgcctcggtcggcgacgacatccgattcggcctcggcgccatccgcaacgtcggcgccaacgtcgtctcgtcactgatcaagacccgcaccgagaagggcaagttcaccgacttctcggactacctcaacaagatcgacatcacggcctgcaacaagaaggtcaccgaatcgctgatcaaggcgggcgctttcgattcgttggggcatccgcgcaagggcctgttcctggtgcacaccgacgccgtcgactcggtgctgggtaccaagaaggccgaggcgatgggggccttcgacctgttcgggggcggcgagg</t>
         </is>
       </c>
     </row>
@@ -628,12 +628,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>F473G-N472F_Block-2</t>
+          <t>F473G_Block-2</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>caacccggagcgtccgtccgcgcccgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgttcggcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
+          <t>cgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacggcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
         </is>
       </c>
     </row>
@@ -645,12 +645,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>E512Q-R517D_Block-2</t>
+          <t>F473G-G474F_Block-2</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>caacccggagcgtccgtccgcgcccgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaagcaggccgccgaggtcgacggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
+          <t>cgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacggcttccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
         </is>
       </c>
     </row>
@@ -662,12 +662,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R517D_Block-2</t>
+          <t>E512Q-R517D_Block-2</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>caacccggagcgtccgtccgcgcccgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtcgacggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
+          <t>cgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaagcaggccgccgaggtcgacggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
         </is>
       </c>
     </row>
@@ -679,12 +679,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>E537R_Block-2</t>
+          <t>R517D_Block-2</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>caacccggagcgtccgtccgcgcccgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctccgcggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
+          <t>cgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtcgacggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
         </is>
       </c>
     </row>
@@ -696,12 +696,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>D643E_Block-2</t>
+          <t>E537R_Block-2</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>caacccggagcgtccgtccgcgcccgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgagggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
+          <t>cgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctccgcggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
         </is>
       </c>
     </row>
@@ -713,12 +713,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>T486-K495_Block-0</t>
+          <t>D643E_Block-2</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ggagatgcctgccatcggcatggaccacgggaacatgttcggcgccagcgagttctacaactcggcgaccaaggccggcatcaaacccatcatcgggatcgaggcctacatcgcgcccggttcccggttcgacaccaagcgcgtcacatggggcgacccgggccagaagggcgacgacgtctccggcagcggtgcgtacacgcacatgacgatggtcgccgagaacgcgacgggcctgcgcaacctgttcaagctgtcctcgctggcgtcgttcgaggggcagctgggcaagtggtcgcgtatggacgccgagatcatcgccgagcacgccgagggcatcatcgccaccaccggctgcccgtcgggcgaggtccagacccgcctgcgcctcggccacgagcgcgaggcgctcgaagccgcggcgaagtggcgcgagatcttcggcccggagaacttcttcctcgaactgatggaccacggtctcgacatcgagcgccgggtccgcgagggcctgctggagatcggccgcaagctcggcatcccgccgctggccaccaacgactgtcactacgtcacgcgtgaggccgcacgcaaccacgaggcgctgctgtgtgtgcagacgggcaagaccctctcggatcccacgcggttcaagttcgacggtgacggctacttcctcaagt</t>
+          <t>cgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgagggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
         </is>
       </c>
     </row>
@@ -730,12 +730,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>D431S-P423D_Block-2</t>
+          <t>P489-K495_Block-2</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>caacccggagcgtccgtccgcggacgatatcgacatcgacttcgactcgcgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
+          <t>cgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
         </is>
       </c>
     </row>
@@ -747,12 +747,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>K826L_Block-4</t>
+          <t>D431S-R432D_Block-2</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ggccaactatccggccgagtacatggcaggcctgctcacctcggtcggtgacgacaaggacctggccgcggtctacctggcggactgccggcgcctgggcatcacggtgctgccgccggacgtcaacgagtcggagcacaacttcgcctcggtcggcgacgacatccgattcggcctcggcgccatccgcaacgtcggcgccaacgtcgtctcgtcactgatcaagacccgcaccgagaagggcaagttcaccgacttctcggactacctcaacaagatcgacatcacggcctgcaacaagaaggtcaccgaatcgctgatcaaggcgggcgctttcgattcgttggggcatccgcgcaagggcctgttcctggtgcacaccgacgccgtcgactcggtgctgggtaccaagaaggccgaggcgatggggcagttcgacctgttcgggggcggcgagg</t>
+          <t>cgatatcgacatcgacttcgactcggaccgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
         </is>
       </c>
     </row>
@@ -764,12 +764,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>I900D_Block-4</t>
+          <t>F862L_Block-4</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ggccaactatccggccgagtacatggcaggcctgctcacctcggtcggtgacgacaaggacaaggccgcggtctacctggcggactgccggcgcctgggcatcacggtgctgccgccggacgtcaacgagtcggagcacaacttcgcctcggtcggcgacgacatccgattcggcctcggcgccatccgcaacgtcggcgccaacgtcgtctcgtcactgatcaagacccgcaccgagaagggcaagttcaccgacttctcggactacctcaacaagatcgacgacacggcctgcaacaagaaggtcaccgaatcgctgatcaaggcgggcgctttcgattcgttggggcatccgcgcaagggcctgttcctggtgcacaccgacgccgtcgactcggtgctgggtaccaagaaggccgaggcgatggggcagttcgacctgttcgggggcggcgagg</t>
+          <t>ggccaactatccggccgagtacatggcaggcctgctcacctcggtcggtgacgacaaggacaaggccgcggtctacctggcggactgccggcgcctgggcatcacggtgctgccgccggacgtcaacgagtcggagcacaacttcgcctcggtcggcgacgacatccgactgggcctcggcgccatccgcaacgtcggcgccaacgtcgtctcgtcactgatcaagacccgcaccgagaagggcaagttcaccgacttctcggactacctcaacaagatcgacatcacggcctgcaacaagaaggtcaccgaatcgctgatcaaggcgggcgctttcgattcgttggggcatccgcgcaagggcctgttcctggtgcacaccgacgccgtcgactcggtgctgggtaccaagaaggccgaggcgatggggcagttcgacctgttcgggggcggcgagg</t>
         </is>
       </c>
     </row>
@@ -781,12 +781,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>L666F_Block-2</t>
+          <t>I900D_Block-4</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>caacccggagcgtccgtccgcgcccgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgttcgcgctgtaccgccccggtccgatgg</t>
+          <t>ggccaactatccggccgagtacatggcaggcctgctcacctcggtcggtgacgacaaggacaaggccgcggtctacctggcggactgccggcgcctgggcatcacggtgctgccgccggacgtcaacgagtcggagcacaacttcgcctcggtcggcgacgacatccgattcggcctcggcgccatccgcaacgtcggcgccaacgtcgtctcgtcactgatcaagacccgcaccgagaagggcaagttcaccgacttctcggactacctcaacaagatcgacgacacggcctgcaacaagaaggtcaccgaatcgctgatcaaggcgggcgctttcgattcgttggggcatccgcgcaagggcctgttcctggtgcacaccgacgccgtcgactcggtgctgggtaccaagaaggccgaggcgatggggcagttcgacctgttcgggggcggcgagg</t>
         </is>
       </c>
     </row>
@@ -798,12 +798,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>R868A_Block-4</t>
+          <t>L666F_Block-2</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ggccaactatccggccgagtacatggcaggcctgctcacctcggtcggtgacgacaaggacaaggccgcggtctacctggcggactgccggcgcctgggcatcacggtgctgccgccggacgtcaacgagtcggagcacaacttcgcctcggtcggcgacgacatccgattcggcctcggcgccatcgccaacgtcggcgccaacgtcgtctcgtcactgatcaagacccgcaccgagaagggcaagttcaccgacttctcggactacctcaacaagatcgacatcacggcctgcaacaagaaggtcaccgaatcgctgatcaaggcgggcgctttcgattcgttggggcatccgcgcaagggcctgttcctggtgcacaccgacgccgtcgactcggtgctgggtaccaagaaggccgaggcgatggggcagttcgacctgttcgggggcggcgagg</t>
+          <t>cgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgttcgcgctgtaccgccccggtccgatgg</t>
         </is>
       </c>
     </row>
@@ -815,12 +815,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>R566A_Block-2</t>
+          <t>R868A_Block-4</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>caacccggagcgtccgtccgcgcccgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaaggccccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
+          <t>ggccaactatccggccgagtacatggcaggcctgctcacctcggtcggtgacgacaaggacaaggccgcggtctacctggcggactgccggcgcctgggcatcacggtgctgccgccggacgtcaacgagtcggagcacaacttcgcctcggtcggcgacgacatccgattcggcctcggcgccatcgccaacgtcggcgccaacgtcgtctcgtcactgatcaagacccgcaccgagaagggcaagttcaccgacttctcggactacctcaacaagatcgacatcacggcctgcaacaagaaggtcaccgaatcgctgatcaaggcgggcgctttcgattcgttggggcatccgcgcaagggcctgttcctggtgcacaccgacgccgtcgactcggtgctgggtaccaagaaggccgaggcgatggggcagttcgacctgttcgggggcggcgagg</t>
         </is>
       </c>
     </row>
@@ -832,12 +832,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>K466A_Block-2</t>
+          <t>R566A_Block-2</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>caacccggagcgtccgtccgcgcccgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctggccgattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
+          <t>cgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaaggccccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
         </is>
       </c>
     </row>
@@ -849,12 +849,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>D467A_Block-2</t>
+          <t>K466A_Block-2</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>caacccggagcgtccgtccgcgcccgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctgaaggcctcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
+          <t>cgatatcgacatcgacttcgacgaccgtcgccgcggcgagatgctgcgctacgccgccaacaggtgggggagcgagcgcgtcgcgcaggtcatcacgttcggcaccatcaagaccaaggcggcgctggccgattcggcccgcgtgaacttcggccagcccggtttcgcgatcgccgaccggatcaccaaggcgctgccgccgcccatcatggccaaggacatcccgctgtcgggtatcaccgacccgaaccacgagcggtacaaggaggccgccgaggtccgcggtctgatcgacaccgatccggacgtgcgcaccatctatgagaccgcgcgcggtctcgaaggcctggtccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagctccgaaccgctcatcgacgcgatcccgctgtggaagcgtccgcaggacggcgcgatcatcaccggctgggactatccgtcgtgtgaggccatcggcctgctgaagatggacttcctgggcctgcgcaacctcacgatcatcggcgacgcgatcgccaacatcaaggccaaccgcggcatcgacctggacctggagacgctgccgctcgacgacccggcggcctacgaattgctctcgcgcggtgacaccctcggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcggcgcatgcagcccacgggcttcaacgacatcgtcgcggtgctcgcgctgtaccgccccggtccgatgg</t>
         </is>
       </c>
     </row>

</xml_diff>